<commit_message>
Updated processing for all years
</commit_message>
<xml_diff>
--- a/data/input/HarvestYear/HY2017/GeneratorForCreateEvals.xlsx
+++ b/data/input/HarvestYear/HY2017/GeneratorForCreateEvals.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Projects\CafPlantGridPointSurvey\ProcessHarvest\data\input\HarvestYear\HY2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A5A905-9A1D-4357-80A7-68100D2A4EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D381FEC4-07D9-41F3-AD4B-D5E89BC1F155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36250" yWindow="-7820" windowWidth="20360" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,13 +80,13 @@
     <t>Reviewer</t>
   </si>
   <si>
-    <t>A decision was made to not harvest at this georeference point even though a crop was planted</t>
-  </si>
-  <si>
     <t>Bryan Carlson</t>
   </si>
   <si>
     <t>Create</t>
+  </si>
+  <si>
+    <t>A decision was made to not collet a sample at this georeference point even though a crop was planted</t>
   </si>
 </sst>
 </file>
@@ -122,9 +122,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,11 +406,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:M88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="Q80" sqref="Q80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="8" max="8" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="86.3046875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -465,28 +468,28 @@
         <v>8</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.CONCAT(B2,C2,"_",A2)</f>
-        <v>CW426_2017</v>
+        <f>_xlfn.CONCAT(B2,C2,"_Bio_",D2,"_",A2)</f>
+        <v>CW426_Bio_SW_2017</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="H2" t="str">
-        <f>_xlfn.CONCAT(B2,C2,"_",A2)</f>
-        <v>CW426_2017</v>
+        <f>_xlfn.CONCAT(B2,C2,"_Bio_",D2,"_",A2)</f>
+        <v>CW426_Bio_SW_2017</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" t="str">
         <f>_xlfn.CONCAT("{""",$A$1,""":",A2,",""",$B$1,""":","""",B2,""",""",$C$1,""":",C2,",""",$D$1,""":""",D2,"""",",""",$E$1,""":""",E2,""",""",$F$1,""":",F2,"}")</f>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":426,"Crop":"SW","SampleId":"CW426_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":426,"Crop":"SW","SampleId":"CW426_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -496,35 +499,35 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>427</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">_xlfn.CONCAT(B3,C3,"_",A3)</f>
-        <v>CW427_2017</v>
+        <f t="shared" ref="E3:E66" si="0">_xlfn.CONCAT(B3,C3,"_Bio_",D3,"_",A3)</f>
+        <v>CW427_Bio_SW_2017</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="1">_xlfn.CONCAT(B3,C3,"_",A3)</f>
-        <v>CW427_2017</v>
+        <f t="shared" ref="H3:H66" si="1">_xlfn.CONCAT(B3,C3,"_Bio_",D3,"_",A3)</f>
+        <v>CW427_Bio_SW_2017</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K66" si="2">_xlfn.CONCAT("{""",$A$1,""":",A3,",""",$B$1,""":","""",B3,""",""",$C$1,""":",C3,",""",$D$1,""":""",D3,"""",",""",$E$1,""":""",E3,""",""",$F$1,""":",F3,"}")</f>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":427,"Crop":"SW","SampleId":"CW427_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":427,"Crop":"SW","SampleId":"CW427_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
@@ -534,7 +537,7 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>428</v>
       </c>
       <c r="D4" t="s">
@@ -542,27 +545,27 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>CW428_2017</v>
+        <v>CW428_Bio_SW_2017</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="1"/>
-        <v>CW428_2017</v>
+        <v>CW428_Bio_SW_2017</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":428,"Crop":"SW","SampleId":"CW428_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":428,"Crop":"SW","SampleId":"CW428_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -572,7 +575,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>429</v>
       </c>
       <c r="D5" t="s">
@@ -580,27 +583,27 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>CW429_2017</v>
+        <v>CW429_Bio_SW_2017</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="1"/>
-        <v>CW429_2017</v>
+        <v>CW429_Bio_SW_2017</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":429,"Crop":"SW","SampleId":"CW429_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":429,"Crop":"SW","SampleId":"CW429_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -610,7 +613,7 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>430</v>
       </c>
       <c r="D6" t="s">
@@ -618,27 +621,27 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>CW430_2017</v>
+        <v>CW430_Bio_SW_2017</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
-        <v>CW430_2017</v>
+        <v>CW430_Bio_SW_2017</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":430,"Crop":"SW","SampleId":"CW430_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":430,"Crop":"SW","SampleId":"CW430_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -648,7 +651,7 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>431</v>
       </c>
       <c r="D7" t="s">
@@ -656,27 +659,27 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>CW431_2017</v>
+        <v>CW431_Bio_SW_2017</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="1"/>
-        <v>CW431_2017</v>
+        <v>CW431_Bio_SW_2017</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":431,"Crop":"SW","SampleId":"CW431_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":431,"Crop":"SW","SampleId":"CW431_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -686,7 +689,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>432</v>
       </c>
       <c r="D8" t="s">
@@ -694,27 +697,27 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>CW432_2017</v>
+        <v>CW432_Bio_SW_2017</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="1"/>
-        <v>CW432_2017</v>
+        <v>CW432_Bio_SW_2017</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":432,"Crop":"SW","SampleId":"CW432_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":432,"Crop":"SW","SampleId":"CW432_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -724,7 +727,7 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>433</v>
       </c>
       <c r="D9" t="s">
@@ -732,27 +735,27 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>CW433_2017</v>
+        <v>CW433_Bio_SW_2017</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="1"/>
-        <v>CW433_2017</v>
+        <v>CW433_Bio_SW_2017</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":433,"Crop":"SW","SampleId":"CW433_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":433,"Crop":"SW","SampleId":"CW433_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -762,7 +765,7 @@
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>434</v>
       </c>
       <c r="D10" t="s">
@@ -770,27 +773,27 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>CW434_2017</v>
+        <v>CW434_Bio_SW_2017</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v>CW434_2017</v>
+        <v>CW434_Bio_SW_2017</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":434,"Crop":"SW","SampleId":"CW434_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":434,"Crop":"SW","SampleId":"CW434_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -800,7 +803,7 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>435</v>
       </c>
       <c r="D11" t="s">
@@ -808,27 +811,27 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>CW435_2017</v>
+        <v>CW435_Bio_SW_2017</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>CW435_2017</v>
+        <v>CW435_Bio_SW_2017</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":435,"Crop":"SW","SampleId":"CW435_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":435,"Crop":"SW","SampleId":"CW435_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -838,7 +841,7 @@
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>436</v>
       </c>
       <c r="D12" t="s">
@@ -846,27 +849,27 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>CW436_2017</v>
+        <v>CW436_Bio_SW_2017</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>CW436_2017</v>
+        <v>CW436_Bio_SW_2017</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":436,"Crop":"SW","SampleId":"CW436_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":436,"Crop":"SW","SampleId":"CW436_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -876,7 +879,7 @@
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>437</v>
       </c>
       <c r="D13" t="s">
@@ -884,27 +887,27 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>CW437_2017</v>
+        <v>CW437_Bio_SW_2017</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>CW437_2017</v>
+        <v>CW437_Bio_SW_2017</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":437,"Crop":"SW","SampleId":"CW437_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":437,"Crop":"SW","SampleId":"CW437_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -914,7 +917,7 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>438</v>
       </c>
       <c r="D14" t="s">
@@ -922,27 +925,27 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>CW438_2017</v>
+        <v>CW438_Bio_SW_2017</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>CW438_2017</v>
+        <v>CW438_Bio_SW_2017</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":438,"Crop":"SW","SampleId":"CW438_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":438,"Crop":"SW","SampleId":"CW438_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -952,7 +955,7 @@
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>439</v>
       </c>
       <c r="D15" t="s">
@@ -960,27 +963,27 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>CW439_2017</v>
+        <v>CW439_Bio_SW_2017</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>CW439_2017</v>
+        <v>CW439_Bio_SW_2017</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":439,"Crop":"SW","SampleId":"CW439_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":439,"Crop":"SW","SampleId":"CW439_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
@@ -990,7 +993,7 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>440</v>
       </c>
       <c r="D16" t="s">
@@ -998,27 +1001,27 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>CW440_2017</v>
+        <v>CW440_Bio_SW_2017</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>CW440_2017</v>
+        <v>CW440_Bio_SW_2017</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":440,"Crop":"SW","SampleId":"CW440_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":440,"Crop":"SW","SampleId":"CW440_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
@@ -1028,7 +1031,7 @@
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>441</v>
       </c>
       <c r="D17" t="s">
@@ -1036,27 +1039,27 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>CW441_2017</v>
+        <v>CW441_Bio_SW_2017</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>CW441_2017</v>
+        <v>CW441_Bio_SW_2017</v>
       </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":441,"Crop":"SW","SampleId":"CW441_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":441,"Crop":"SW","SampleId":"CW441_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
@@ -1066,7 +1069,7 @@
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>442</v>
       </c>
       <c r="D18" t="s">
@@ -1074,27 +1077,27 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>CW442_2017</v>
+        <v>CW442_Bio_SW_2017</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>CW442_2017</v>
+        <v>CW442_Bio_SW_2017</v>
       </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":442,"Crop":"SW","SampleId":"CW442_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":442,"Crop":"SW","SampleId":"CW442_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
@@ -1104,7 +1107,7 @@
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>443</v>
       </c>
       <c r="D19" t="s">
@@ -1112,27 +1115,27 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>CW443_2017</v>
+        <v>CW443_Bio_SW_2017</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>CW443_2017</v>
+        <v>CW443_Bio_SW_2017</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":443,"Crop":"SW","SampleId":"CW443_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":443,"Crop":"SW","SampleId":"CW443_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
@@ -1142,7 +1145,7 @@
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>444</v>
       </c>
       <c r="D20" t="s">
@@ -1150,27 +1153,27 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>CW444_2017</v>
+        <v>CW444_Bio_SW_2017</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>CW444_2017</v>
+        <v>CW444_Bio_SW_2017</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":444,"Crop":"SW","SampleId":"CW444_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":444,"Crop":"SW","SampleId":"CW444_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
@@ -1180,7 +1183,7 @@
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>445</v>
       </c>
       <c r="D21" t="s">
@@ -1188,27 +1191,27 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>CW445_2017</v>
+        <v>CW445_Bio_SW_2017</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>CW445_2017</v>
+        <v>CW445_Bio_SW_2017</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":445,"Crop":"SW","SampleId":"CW445_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":445,"Crop":"SW","SampleId":"CW445_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
@@ -1218,7 +1221,7 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>446</v>
       </c>
       <c r="D22" t="s">
@@ -1226,27 +1229,27 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>CW446_2017</v>
+        <v>CW446_Bio_SW_2017</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>CW446_2017</v>
+        <v>CW446_Bio_SW_2017</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":446,"Crop":"SW","SampleId":"CW446_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":446,"Crop":"SW","SampleId":"CW446_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
@@ -1256,7 +1259,7 @@
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>447</v>
       </c>
       <c r="D23" t="s">
@@ -1264,27 +1267,27 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>CW447_2017</v>
+        <v>CW447_Bio_SW_2017</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v>CW447_2017</v>
+        <v>CW447_Bio_SW_2017</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":447,"Crop":"SW","SampleId":"CW447_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":447,"Crop":"SW","SampleId":"CW447_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
@@ -1294,7 +1297,7 @@
       <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>448</v>
       </c>
       <c r="D24" t="s">
@@ -1302,27 +1305,27 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>CW448_2017</v>
+        <v>CW448_Bio_SW_2017</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>CW448_2017</v>
+        <v>CW448_Bio_SW_2017</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":448,"Crop":"SW","SampleId":"CW448_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":448,"Crop":"SW","SampleId":"CW448_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L24" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
@@ -1332,7 +1335,7 @@
       <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>449</v>
       </c>
       <c r="D25" t="s">
@@ -1340,27 +1343,27 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>CW449_2017</v>
+        <v>CW449_Bio_SW_2017</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>CW449_2017</v>
+        <v>CW449_Bio_SW_2017</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":449,"Crop":"SW","SampleId":"CW449_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":449,"Crop":"SW","SampleId":"CW449_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.4">
@@ -1370,7 +1373,7 @@
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>450</v>
       </c>
       <c r="D26" t="s">
@@ -1378,27 +1381,27 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>CW450_2017</v>
+        <v>CW450_Bio_SW_2017</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>CW450_2017</v>
+        <v>CW450_Bio_SW_2017</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":450,"Crop":"SW","SampleId":"CW450_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":450,"Crop":"SW","SampleId":"CW450_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.4">
@@ -1408,7 +1411,7 @@
       <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>451</v>
       </c>
       <c r="D27" t="s">
@@ -1416,27 +1419,27 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>CW451_2017</v>
+        <v>CW451_Bio_SW_2017</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>CW451_2017</v>
+        <v>CW451_Bio_SW_2017</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":451,"Crop":"SW","SampleId":"CW451_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":451,"Crop":"SW","SampleId":"CW451_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.4">
@@ -1446,7 +1449,7 @@
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>452</v>
       </c>
       <c r="D28" t="s">
@@ -1454,27 +1457,27 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>CW452_2017</v>
+        <v>CW452_Bio_SW_2017</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>CW452_2017</v>
+        <v>CW452_Bio_SW_2017</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":452,"Crop":"SW","SampleId":"CW452_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":452,"Crop":"SW","SampleId":"CW452_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.4">
@@ -1484,7 +1487,7 @@
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>453</v>
       </c>
       <c r="D29" t="s">
@@ -1492,27 +1495,27 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>CW453_2017</v>
+        <v>CW453_Bio_SW_2017</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>CW453_2017</v>
+        <v>CW453_Bio_SW_2017</v>
       </c>
       <c r="I29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":453,"Crop":"SW","SampleId":"CW453_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":453,"Crop":"SW","SampleId":"CW453_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.4">
@@ -1522,7 +1525,7 @@
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>454</v>
       </c>
       <c r="D30" t="s">
@@ -1530,27 +1533,27 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>CW454_2017</v>
+        <v>CW454_Bio_SW_2017</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>CW454_2017</v>
+        <v>CW454_Bio_SW_2017</v>
       </c>
       <c r="I30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":454,"Crop":"SW","SampleId":"CW454_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":454,"Crop":"SW","SampleId":"CW454_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
@@ -1560,7 +1563,7 @@
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>455</v>
       </c>
       <c r="D31" t="s">
@@ -1568,27 +1571,27 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>CW455_2017</v>
+        <v>CW455_Bio_SW_2017</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
-        <v>CW455_2017</v>
+        <v>CW455_Bio_SW_2017</v>
       </c>
       <c r="I31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":455,"Crop":"SW","SampleId":"CW455_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":455,"Crop":"SW","SampleId":"CW455_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
@@ -1598,7 +1601,7 @@
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>456</v>
       </c>
       <c r="D32" t="s">
@@ -1606,27 +1609,27 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>CW456_2017</v>
+        <v>CW456_Bio_SW_2017</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
-        <v>CW456_2017</v>
+        <v>CW456_Bio_SW_2017</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":456,"Crop":"SW","SampleId":"CW456_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":456,"Crop":"SW","SampleId":"CW456_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
@@ -1636,7 +1639,7 @@
       <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>457</v>
       </c>
       <c r="D33" t="s">
@@ -1644,27 +1647,27 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>CW457_2017</v>
+        <v>CW457_Bio_SW_2017</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
-        <v>CW457_2017</v>
+        <v>CW457_Bio_SW_2017</v>
       </c>
       <c r="I33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":457,"Crop":"SW","SampleId":"CW457_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":457,"Crop":"SW","SampleId":"CW457_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
@@ -1674,7 +1677,7 @@
       <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>458</v>
       </c>
       <c r="D34" t="s">
@@ -1682,27 +1685,27 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>CW458_2017</v>
+        <v>CW458_Bio_SW_2017</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
-        <v>CW458_2017</v>
+        <v>CW458_Bio_SW_2017</v>
       </c>
       <c r="I34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":458,"Crop":"SW","SampleId":"CW458_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":458,"Crop":"SW","SampleId":"CW458_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L34" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.4">
@@ -1712,7 +1715,7 @@
       <c r="B35" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>459</v>
       </c>
       <c r="D35" t="s">
@@ -1720,27 +1723,27 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>CW459_2017</v>
+        <v>CW459_Bio_SW_2017</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
-        <v>CW459_2017</v>
+        <v>CW459_Bio_SW_2017</v>
       </c>
       <c r="I35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":459,"Crop":"SW","SampleId":"CW459_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":459,"Crop":"SW","SampleId":"CW459_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L35" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.4">
@@ -1750,7 +1753,7 @@
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>460</v>
       </c>
       <c r="D36" t="s">
@@ -1758,27 +1761,27 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>CW460_2017</v>
+        <v>CW460_Bio_SW_2017</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
-        <v>CW460_2017</v>
+        <v>CW460_Bio_SW_2017</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":460,"Crop":"SW","SampleId":"CW460_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":460,"Crop":"SW","SampleId":"CW460_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L36" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.4">
@@ -1788,7 +1791,7 @@
       <c r="B37" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>461</v>
       </c>
       <c r="D37" t="s">
@@ -1796,27 +1799,27 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>CW461_2017</v>
+        <v>CW461_Bio_SW_2017</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
-        <v>CW461_2017</v>
+        <v>CW461_Bio_SW_2017</v>
       </c>
       <c r="I37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":461,"Crop":"SW","SampleId":"CW461_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":461,"Crop":"SW","SampleId":"CW461_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L37" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.4">
@@ -1826,7 +1829,7 @@
       <c r="B38" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>462</v>
       </c>
       <c r="D38" t="s">
@@ -1834,27 +1837,27 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>CW462_2017</v>
+        <v>CW462_Bio_SW_2017</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
-        <v>CW462_2017</v>
+        <v>CW462_Bio_SW_2017</v>
       </c>
       <c r="I38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":462,"Crop":"SW","SampleId":"CW462_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":462,"Crop":"SW","SampleId":"CW462_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L38" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.4">
@@ -1864,7 +1867,7 @@
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>463</v>
       </c>
       <c r="D39" t="s">
@@ -1872,27 +1875,27 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>CW463_2017</v>
+        <v>CW463_Bio_SW_2017</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
-        <v>CW463_2017</v>
+        <v>CW463_Bio_SW_2017</v>
       </c>
       <c r="I39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":463,"Crop":"SW","SampleId":"CW463_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":463,"Crop":"SW","SampleId":"CW463_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.4">
@@ -1902,7 +1905,7 @@
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40">
         <v>464</v>
       </c>
       <c r="D40" t="s">
@@ -1910,27 +1913,27 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>CW464_2017</v>
+        <v>CW464_Bio_SW_2017</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="1"/>
-        <v>CW464_2017</v>
+        <v>CW464_Bio_SW_2017</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":464,"Crop":"SW","SampleId":"CW464_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":464,"Crop":"SW","SampleId":"CW464_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L40" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.4">
@@ -1940,7 +1943,7 @@
       <c r="B41" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>465</v>
       </c>
       <c r="D41" t="s">
@@ -1948,27 +1951,27 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>CW465_2017</v>
+        <v>CW465_Bio_SW_2017</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="1"/>
-        <v>CW465_2017</v>
+        <v>CW465_Bio_SW_2017</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":465,"Crop":"SW","SampleId":"CW465_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":465,"Crop":"SW","SampleId":"CW465_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L41" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.4">
@@ -1978,7 +1981,7 @@
       <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42">
         <v>466</v>
       </c>
       <c r="D42" t="s">
@@ -1986,27 +1989,27 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>CW466_2017</v>
+        <v>CW466_Bio_SW_2017</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="1"/>
-        <v>CW466_2017</v>
+        <v>CW466_Bio_SW_2017</v>
       </c>
       <c r="I42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":466,"Crop":"SW","SampleId":"CW466_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":466,"Crop":"SW","SampleId":"CW466_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L42" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.4">
@@ -2016,7 +2019,7 @@
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
         <v>467</v>
       </c>
       <c r="D43" t="s">
@@ -2024,27 +2027,27 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>CW467_2017</v>
+        <v>CW467_Bio_SW_2017</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="1"/>
-        <v>CW467_2017</v>
+        <v>CW467_Bio_SW_2017</v>
       </c>
       <c r="I43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":467,"Crop":"SW","SampleId":"CW467_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":467,"Crop":"SW","SampleId":"CW467_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L43" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.4">
@@ -2054,7 +2057,7 @@
       <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>468</v>
       </c>
       <c r="D44" t="s">
@@ -2062,27 +2065,27 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>CW468_2017</v>
+        <v>CW468_Bio_SW_2017</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="1"/>
-        <v>CW468_2017</v>
+        <v>CW468_Bio_SW_2017</v>
       </c>
       <c r="I44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":468,"Crop":"SW","SampleId":"CW468_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":468,"Crop":"SW","SampleId":"CW468_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L44" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.4">
@@ -2092,7 +2095,7 @@
       <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>469</v>
       </c>
       <c r="D45" t="s">
@@ -2100,27 +2103,27 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>CW469_2017</v>
+        <v>CW469_Bio_SW_2017</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="1"/>
-        <v>CW469_2017</v>
+        <v>CW469_Bio_SW_2017</v>
       </c>
       <c r="I45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":469,"Crop":"SW","SampleId":"CW469_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":469,"Crop":"SW","SampleId":"CW469_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L45" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.4">
@@ -2130,7 +2133,7 @@
       <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
         <v>470</v>
       </c>
       <c r="D46" t="s">
@@ -2138,27 +2141,27 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>CW470_2017</v>
+        <v>CW470_Bio_SW_2017</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="1"/>
-        <v>CW470_2017</v>
+        <v>CW470_Bio_SW_2017</v>
       </c>
       <c r="I46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":470,"Crop":"SW","SampleId":"CW470_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":470,"Crop":"SW","SampleId":"CW470_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L46" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.4">
@@ -2168,7 +2171,7 @@
       <c r="B47" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>472</v>
       </c>
       <c r="D47" t="s">
@@ -2176,27 +2179,27 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>CW472_2017</v>
+        <v>CW472_Bio_SW_2017</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="1"/>
-        <v>CW472_2017</v>
+        <v>CW472_Bio_SW_2017</v>
       </c>
       <c r="I47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":472,"Crop":"SW","SampleId":"CW472_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":472,"Crop":"SW","SampleId":"CW472_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L47" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.4">
@@ -2206,7 +2209,7 @@
       <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>473</v>
       </c>
       <c r="D48" t="s">
@@ -2214,27 +2217,27 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>CW473_2017</v>
+        <v>CW473_Bio_SW_2017</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="1"/>
-        <v>CW473_2017</v>
+        <v>CW473_Bio_SW_2017</v>
       </c>
       <c r="I48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":473,"Crop":"SW","SampleId":"CW473_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":473,"Crop":"SW","SampleId":"CW473_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L48" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.4">
@@ -2244,7 +2247,7 @@
       <c r="B49" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>474</v>
       </c>
       <c r="D49" t="s">
@@ -2252,27 +2255,27 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>CW474_2017</v>
+        <v>CW474_Bio_SW_2017</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="1"/>
-        <v>CW474_2017</v>
+        <v>CW474_Bio_SW_2017</v>
       </c>
       <c r="I49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":474,"Crop":"SW","SampleId":"CW474_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":474,"Crop":"SW","SampleId":"CW474_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.4">
@@ -2282,7 +2285,7 @@
       <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
         <v>475</v>
       </c>
       <c r="D50" t="s">
@@ -2290,27 +2293,27 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>CW475_2017</v>
+        <v>CW475_Bio_SW_2017</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="1"/>
-        <v>CW475_2017</v>
+        <v>CW475_Bio_SW_2017</v>
       </c>
       <c r="I50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":475,"Crop":"SW","SampleId":"CW475_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":475,"Crop":"SW","SampleId":"CW475_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L50" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.4">
@@ -2320,7 +2323,7 @@
       <c r="B51" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51">
         <v>476</v>
       </c>
       <c r="D51" t="s">
@@ -2328,27 +2331,27 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>CW476_2017</v>
+        <v>CW476_Bio_SW_2017</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="1"/>
-        <v>CW476_2017</v>
+        <v>CW476_Bio_SW_2017</v>
       </c>
       <c r="I51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":476,"Crop":"SW","SampleId":"CW476_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":476,"Crop":"SW","SampleId":"CW476_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L51" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.4">
@@ -2358,7 +2361,7 @@
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52">
         <v>477</v>
       </c>
       <c r="D52" t="s">
@@ -2366,27 +2369,27 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>CW477_2017</v>
+        <v>CW477_Bio_SW_2017</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="1"/>
-        <v>CW477_2017</v>
+        <v>CW477_Bio_SW_2017</v>
       </c>
       <c r="I52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":477,"Crop":"SW","SampleId":"CW477_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":477,"Crop":"SW","SampleId":"CW477_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L52" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.4">
@@ -2396,7 +2399,7 @@
       <c r="B53" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53">
         <v>478</v>
       </c>
       <c r="D53" t="s">
@@ -2404,27 +2407,27 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>CW478_2017</v>
+        <v>CW478_Bio_SW_2017</v>
       </c>
       <c r="F53">
         <v>1</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="1"/>
-        <v>CW478_2017</v>
+        <v>CW478_Bio_SW_2017</v>
       </c>
       <c r="I53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":478,"Crop":"SW","SampleId":"CW478_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":478,"Crop":"SW","SampleId":"CW478_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L53" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.4">
@@ -2434,7 +2437,7 @@
       <c r="B54" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54">
         <v>479</v>
       </c>
       <c r="D54" t="s">
@@ -2442,27 +2445,27 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>CW479_2017</v>
+        <v>CW479_Bio_SW_2017</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="1"/>
-        <v>CW479_2017</v>
+        <v>CW479_Bio_SW_2017</v>
       </c>
       <c r="I54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":479,"Crop":"SW","SampleId":"CW479_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":479,"Crop":"SW","SampleId":"CW479_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L54" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.4">
@@ -2472,7 +2475,7 @@
       <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
         <v>480</v>
       </c>
       <c r="D55" t="s">
@@ -2480,27 +2483,27 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>CW480_2017</v>
+        <v>CW480_Bio_SW_2017</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="1"/>
-        <v>CW480_2017</v>
+        <v>CW480_Bio_SW_2017</v>
       </c>
       <c r="I55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":480,"Crop":"SW","SampleId":"CW480_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":480,"Crop":"SW","SampleId":"CW480_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L55" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.4">
@@ -2510,7 +2513,7 @@
       <c r="B56" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56">
         <v>483</v>
       </c>
       <c r="D56" t="s">
@@ -2518,27 +2521,27 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>CW483_2017</v>
+        <v>CW483_Bio_SW_2017</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="1"/>
-        <v>CW483_2017</v>
+        <v>CW483_Bio_SW_2017</v>
       </c>
       <c r="I56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":483,"Crop":"SW","SampleId":"CW483_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":483,"Crop":"SW","SampleId":"CW483_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L56" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.4">
@@ -2548,7 +2551,7 @@
       <c r="B57" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
         <v>484</v>
       </c>
       <c r="D57" t="s">
@@ -2556,27 +2559,27 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>CW484_2017</v>
+        <v>CW484_Bio_SW_2017</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="1"/>
-        <v>CW484_2017</v>
+        <v>CW484_Bio_SW_2017</v>
       </c>
       <c r="I57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":484,"Crop":"SW","SampleId":"CW484_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":484,"Crop":"SW","SampleId":"CW484_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L57" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
@@ -2586,7 +2589,7 @@
       <c r="B58" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
         <v>485</v>
       </c>
       <c r="D58" t="s">
@@ -2594,27 +2597,27 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>CW485_2017</v>
+        <v>CW485_Bio_SW_2017</v>
       </c>
       <c r="F58">
         <v>1</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="1"/>
-        <v>CW485_2017</v>
+        <v>CW485_Bio_SW_2017</v>
       </c>
       <c r="I58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":485,"Crop":"SW","SampleId":"CW485_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":485,"Crop":"SW","SampleId":"CW485_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L58" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.4">
@@ -2624,7 +2627,7 @@
       <c r="B59" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
         <v>486</v>
       </c>
       <c r="D59" t="s">
@@ -2632,27 +2635,27 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>CW486_2017</v>
+        <v>CW486_Bio_SW_2017</v>
       </c>
       <c r="F59">
         <v>1</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="1"/>
-        <v>CW486_2017</v>
+        <v>CW486_Bio_SW_2017</v>
       </c>
       <c r="I59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":486,"Crop":"SW","SampleId":"CW486_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":486,"Crop":"SW","SampleId":"CW486_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L59" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
@@ -2662,7 +2665,7 @@
       <c r="B60" t="s">
         <v>7</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
         <v>487</v>
       </c>
       <c r="D60" t="s">
@@ -2670,27 +2673,27 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>CW487_2017</v>
+        <v>CW487_Bio_SW_2017</v>
       </c>
       <c r="F60">
         <v>1</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="1"/>
-        <v>CW487_2017</v>
+        <v>CW487_Bio_SW_2017</v>
       </c>
       <c r="I60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":487,"Crop":"SW","SampleId":"CW487_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":487,"Crop":"SW","SampleId":"CW487_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L60" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
@@ -2700,7 +2703,7 @@
       <c r="B61" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
         <v>488</v>
       </c>
       <c r="D61" t="s">
@@ -2708,27 +2711,27 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>CW488_2017</v>
+        <v>CW488_Bio_SW_2017</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="1"/>
-        <v>CW488_2017</v>
+        <v>CW488_Bio_SW_2017</v>
       </c>
       <c r="I61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":488,"Crop":"SW","SampleId":"CW488_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":488,"Crop":"SW","SampleId":"CW488_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L61" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.4">
@@ -2738,7 +2741,7 @@
       <c r="B62" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
         <v>489</v>
       </c>
       <c r="D62" t="s">
@@ -2746,27 +2749,27 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>CW489_2017</v>
+        <v>CW489_Bio_SW_2017</v>
       </c>
       <c r="F62">
         <v>1</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="1"/>
-        <v>CW489_2017</v>
+        <v>CW489_Bio_SW_2017</v>
       </c>
       <c r="I62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":489,"Crop":"SW","SampleId":"CW489_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":489,"Crop":"SW","SampleId":"CW489_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L62" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
@@ -2776,7 +2779,7 @@
       <c r="B63" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
         <v>490</v>
       </c>
       <c r="D63" t="s">
@@ -2784,27 +2787,27 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>CW490_2017</v>
+        <v>CW490_Bio_SW_2017</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="1"/>
-        <v>CW490_2017</v>
+        <v>CW490_Bio_SW_2017</v>
       </c>
       <c r="I63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":490,"Crop":"SW","SampleId":"CW490_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":490,"Crop":"SW","SampleId":"CW490_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L63" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
@@ -2814,7 +2817,7 @@
       <c r="B64" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
         <v>491</v>
       </c>
       <c r="D64" t="s">
@@ -2822,27 +2825,27 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>CW491_2017</v>
+        <v>CW491_Bio_SW_2017</v>
       </c>
       <c r="F64">
         <v>1</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="1"/>
-        <v>CW491_2017</v>
+        <v>CW491_Bio_SW_2017</v>
       </c>
       <c r="I64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":491,"Crop":"SW","SampleId":"CW491_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":491,"Crop":"SW","SampleId":"CW491_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L64" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
@@ -2852,7 +2855,7 @@
       <c r="B65" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>492</v>
       </c>
       <c r="D65" t="s">
@@ -2860,27 +2863,27 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>CW492_2017</v>
+        <v>CW492_Bio_SW_2017</v>
       </c>
       <c r="F65">
         <v>1</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="1"/>
-        <v>CW492_2017</v>
+        <v>CW492_Bio_SW_2017</v>
       </c>
       <c r="I65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":492,"Crop":"SW","SampleId":"CW492_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":492,"Crop":"SW","SampleId":"CW492_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L65" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
@@ -2890,7 +2893,7 @@
       <c r="B66" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66">
         <v>493</v>
       </c>
       <c r="D66" t="s">
@@ -2898,27 +2901,27 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>CW493_2017</v>
+        <v>CW493_Bio_SW_2017</v>
       </c>
       <c r="F66">
         <v>1</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="1"/>
-        <v>CW493_2017</v>
+        <v>CW493_Bio_SW_2017</v>
       </c>
       <c r="I66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="2"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":493,"Crop":"SW","SampleId":"CW493_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":493,"Crop":"SW","SampleId":"CW493_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L66" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
@@ -2928,35 +2931,35 @@
       <c r="B67" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67">
         <v>497</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E88" si="3">_xlfn.CONCAT(B67,C67,"_",A67)</f>
-        <v>CW497_2017</v>
+        <f t="shared" ref="E67:E88" si="3">_xlfn.CONCAT(B67,C67,"_Bio_",D67,"_",A67)</f>
+        <v>CW497_Bio_SW_2017</v>
       </c>
       <c r="F67">
         <v>1</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H88" si="4">_xlfn.CONCAT(B67,C67,"_",A67)</f>
-        <v>CW497_2017</v>
+        <f t="shared" ref="H67:H88" si="4">_xlfn.CONCAT(B67,C67,"_Bio_",D67,"_",A67)</f>
+        <v>CW497_Bio_SW_2017</v>
       </c>
       <c r="I67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" ref="K67:K88" si="5">_xlfn.CONCAT("{""",$A$1,""":",A67,",""",$B$1,""":","""",B67,""",""",$C$1,""":",C67,",""",$D$1,""":""",D67,"""",",""",$E$1,""":""",E67,""",""",$F$1,""":",F67,"}")</f>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":497,"Crop":"SW","SampleId":"CW497_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":497,"Crop":"SW","SampleId":"CW497_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L67" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.4">
@@ -2966,7 +2969,7 @@
       <c r="B68" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68">
         <v>498</v>
       </c>
       <c r="D68" t="s">
@@ -2974,27 +2977,27 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="3"/>
-        <v>CW498_2017</v>
+        <v>CW498_Bio_SW_2017</v>
       </c>
       <c r="F68">
         <v>1</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="4"/>
-        <v>CW498_2017</v>
+        <v>CW498_Bio_SW_2017</v>
       </c>
       <c r="I68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":498,"Crop":"SW","SampleId":"CW498_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":498,"Crop":"SW","SampleId":"CW498_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L68" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
@@ -3004,7 +3007,7 @@
       <c r="B69" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C69">
         <v>499</v>
       </c>
       <c r="D69" t="s">
@@ -3012,27 +3015,27 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>CW499_2017</v>
+        <v>CW499_Bio_SW_2017</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="4"/>
-        <v>CW499_2017</v>
+        <v>CW499_Bio_SW_2017</v>
       </c>
       <c r="I69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":499,"Crop":"SW","SampleId":"CW499_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":499,"Crop":"SW","SampleId":"CW499_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L69" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
@@ -3042,7 +3045,7 @@
       <c r="B70" t="s">
         <v>7</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70">
         <v>500</v>
       </c>
       <c r="D70" t="s">
@@ -3050,27 +3053,27 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>CW500_2017</v>
+        <v>CW500_Bio_SW_2017</v>
       </c>
       <c r="F70">
         <v>1</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="4"/>
-        <v>CW500_2017</v>
+        <v>CW500_Bio_SW_2017</v>
       </c>
       <c r="I70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":500,"Crop":"SW","SampleId":"CW500_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":500,"Crop":"SW","SampleId":"CW500_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L70" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
@@ -3080,7 +3083,7 @@
       <c r="B71" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C71">
         <v>501</v>
       </c>
       <c r="D71" t="s">
@@ -3088,27 +3091,27 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>CW501_2017</v>
+        <v>CW501_Bio_SW_2017</v>
       </c>
       <c r="F71">
         <v>1</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="4"/>
-        <v>CW501_2017</v>
+        <v>CW501_Bio_SW_2017</v>
       </c>
       <c r="I71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":501,"Crop":"SW","SampleId":"CW501_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":501,"Crop":"SW","SampleId":"CW501_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L71" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
@@ -3118,7 +3121,7 @@
       <c r="B72" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72">
         <v>502</v>
       </c>
       <c r="D72" t="s">
@@ -3126,27 +3129,27 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="3"/>
-        <v>CW502_2017</v>
+        <v>CW502_Bio_SW_2017</v>
       </c>
       <c r="F72">
         <v>1</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="4"/>
-        <v>CW502_2017</v>
+        <v>CW502_Bio_SW_2017</v>
       </c>
       <c r="I72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":502,"Crop":"SW","SampleId":"CW502_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":502,"Crop":"SW","SampleId":"CW502_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L72" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
@@ -3156,7 +3159,7 @@
       <c r="B73" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73">
         <v>503</v>
       </c>
       <c r="D73" t="s">
@@ -3164,27 +3167,27 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="3"/>
-        <v>CW503_2017</v>
+        <v>CW503_Bio_SW_2017</v>
       </c>
       <c r="F73">
         <v>1</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="4"/>
-        <v>CW503_2017</v>
+        <v>CW503_Bio_SW_2017</v>
       </c>
       <c r="I73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":503,"Crop":"SW","SampleId":"CW503_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":503,"Crop":"SW","SampleId":"CW503_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L73" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
@@ -3194,7 +3197,7 @@
       <c r="B74" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74">
         <v>504</v>
       </c>
       <c r="D74" t="s">
@@ -3202,27 +3205,27 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="3"/>
-        <v>CW504_2017</v>
+        <v>CW504_Bio_SW_2017</v>
       </c>
       <c r="F74">
         <v>1</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="4"/>
-        <v>CW504_2017</v>
+        <v>CW504_Bio_SW_2017</v>
       </c>
       <c r="I74" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":504,"Crop":"SW","SampleId":"CW504_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":504,"Crop":"SW","SampleId":"CW504_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L74" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.4">
@@ -3232,7 +3235,7 @@
       <c r="B75" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75">
         <v>505</v>
       </c>
       <c r="D75" t="s">
@@ -3240,27 +3243,27 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="3"/>
-        <v>CW505_2017</v>
+        <v>CW505_Bio_SW_2017</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="4"/>
-        <v>CW505_2017</v>
+        <v>CW505_Bio_SW_2017</v>
       </c>
       <c r="I75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":505,"Crop":"SW","SampleId":"CW505_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":505,"Crop":"SW","SampleId":"CW505_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L75" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.4">
@@ -3270,7 +3273,7 @@
       <c r="B76" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C76">
         <v>506</v>
       </c>
       <c r="D76" t="s">
@@ -3278,27 +3281,27 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="3"/>
-        <v>CW506_2017</v>
+        <v>CW506_Bio_SW_2017</v>
       </c>
       <c r="F76">
         <v>1</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="4"/>
-        <v>CW506_2017</v>
+        <v>CW506_Bio_SW_2017</v>
       </c>
       <c r="I76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":506,"Crop":"SW","SampleId":"CW506_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":506,"Crop":"SW","SampleId":"CW506_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L76" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.4">
@@ -3308,7 +3311,7 @@
       <c r="B77" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77">
         <v>511</v>
       </c>
       <c r="D77" t="s">
@@ -3316,27 +3319,27 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
-        <v>CW511_2017</v>
+        <v>CW511_Bio_SW_2017</v>
       </c>
       <c r="F77">
         <v>1</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="4"/>
-        <v>CW511_2017</v>
+        <v>CW511_Bio_SW_2017</v>
       </c>
       <c r="I77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":511,"Crop":"SW","SampleId":"CW511_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":511,"Crop":"SW","SampleId":"CW511_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L77" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
@@ -3346,7 +3349,7 @@
       <c r="B78" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78">
         <v>512</v>
       </c>
       <c r="D78" t="s">
@@ -3354,27 +3357,27 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
-        <v>CW512_2017</v>
+        <v>CW512_Bio_SW_2017</v>
       </c>
       <c r="F78">
         <v>1</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="4"/>
-        <v>CW512_2017</v>
+        <v>CW512_Bio_SW_2017</v>
       </c>
       <c r="I78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":512,"Crop":"SW","SampleId":"CW512_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":512,"Crop":"SW","SampleId":"CW512_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L78" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.4">
@@ -3384,7 +3387,7 @@
       <c r="B79" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79">
         <v>513</v>
       </c>
       <c r="D79" t="s">
@@ -3392,27 +3395,27 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
-        <v>CW513_2017</v>
+        <v>CW513_Bio_SW_2017</v>
       </c>
       <c r="F79">
         <v>1</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="4"/>
-        <v>CW513_2017</v>
+        <v>CW513_Bio_SW_2017</v>
       </c>
       <c r="I79" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":513,"Crop":"SW","SampleId":"CW513_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":513,"Crop":"SW","SampleId":"CW513_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L79" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.4">
@@ -3422,7 +3425,7 @@
       <c r="B80" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80">
         <v>514</v>
       </c>
       <c r="D80" t="s">
@@ -3430,27 +3433,27 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
-        <v>CW514_2017</v>
+        <v>CW514_Bio_SW_2017</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="4"/>
-        <v>CW514_2017</v>
+        <v>CW514_Bio_SW_2017</v>
       </c>
       <c r="I80" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":514,"Crop":"SW","SampleId":"CW514_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":514,"Crop":"SW","SampleId":"CW514_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L80" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.4">
@@ -3460,7 +3463,7 @@
       <c r="B81" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81">
         <v>515</v>
       </c>
       <c r="D81" t="s">
@@ -3468,27 +3471,27 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>CW515_2017</v>
+        <v>CW515_Bio_SW_2017</v>
       </c>
       <c r="F81">
         <v>1</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="4"/>
-        <v>CW515_2017</v>
+        <v>CW515_Bio_SW_2017</v>
       </c>
       <c r="I81" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":515,"Crop":"SW","SampleId":"CW515_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":515,"Crop":"SW","SampleId":"CW515_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L81" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
@@ -3498,7 +3501,7 @@
       <c r="B82" t="s">
         <v>7</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82">
         <v>516</v>
       </c>
       <c r="D82" t="s">
@@ -3506,27 +3509,27 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
-        <v>CW516_2017</v>
+        <v>CW516_Bio_SW_2017</v>
       </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="4"/>
-        <v>CW516_2017</v>
+        <v>CW516_Bio_SW_2017</v>
       </c>
       <c r="I82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":516,"Crop":"SW","SampleId":"CW516_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":516,"Crop":"SW","SampleId":"CW516_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L82" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.4">
@@ -3536,7 +3539,7 @@
       <c r="B83" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83">
         <v>517</v>
       </c>
       <c r="D83" t="s">
@@ -3544,27 +3547,27 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="3"/>
-        <v>CW517_2017</v>
+        <v>CW517_Bio_SW_2017</v>
       </c>
       <c r="F83">
         <v>1</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="4"/>
-        <v>CW517_2017</v>
+        <v>CW517_Bio_SW_2017</v>
       </c>
       <c r="I83" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":517,"Crop":"SW","SampleId":"CW517_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":517,"Crop":"SW","SampleId":"CW517_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L83" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.4">
@@ -3574,7 +3577,7 @@
       <c r="B84" t="s">
         <v>7</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84">
         <v>518</v>
       </c>
       <c r="D84" t="s">
@@ -3582,27 +3585,27 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
-        <v>CW518_2017</v>
+        <v>CW518_Bio_SW_2017</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="4"/>
-        <v>CW518_2017</v>
+        <v>CW518_Bio_SW_2017</v>
       </c>
       <c r="I84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":518,"Crop":"SW","SampleId":"CW518_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":518,"Crop":"SW","SampleId":"CW518_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L84" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.4">
@@ -3612,7 +3615,7 @@
       <c r="B85" t="s">
         <v>7</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85">
         <v>519</v>
       </c>
       <c r="D85" t="s">
@@ -3620,27 +3623,27 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
-        <v>CW519_2017</v>
+        <v>CW519_Bio_SW_2017</v>
       </c>
       <c r="F85">
         <v>1</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="4"/>
-        <v>CW519_2017</v>
+        <v>CW519_Bio_SW_2017</v>
       </c>
       <c r="I85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":519,"Crop":"SW","SampleId":"CW519_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":519,"Crop":"SW","SampleId":"CW519_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L85" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.4">
@@ -3650,7 +3653,7 @@
       <c r="B86" t="s">
         <v>7</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86">
         <v>528</v>
       </c>
       <c r="D86" t="s">
@@ -3658,27 +3661,27 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
-        <v>CW528_2017</v>
+        <v>CW528_Bio_SW_2017</v>
       </c>
       <c r="F86">
         <v>1</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="4"/>
-        <v>CW528_2017</v>
+        <v>CW528_Bio_SW_2017</v>
       </c>
       <c r="I86" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":528,"Crop":"SW","SampleId":"CW528_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":528,"Crop":"SW","SampleId":"CW528_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L86" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.4">
@@ -3688,7 +3691,7 @@
       <c r="B87" t="s">
         <v>7</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C87">
         <v>529</v>
       </c>
       <c r="D87" t="s">
@@ -3696,27 +3699,27 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
-        <v>CW529_2017</v>
+        <v>CW529_Bio_SW_2017</v>
       </c>
       <c r="F87">
         <v>1</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="4"/>
-        <v>CW529_2017</v>
+        <v>CW529_Bio_SW_2017</v>
       </c>
       <c r="I87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":529,"Crop":"SW","SampleId":"CW529_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":529,"Crop":"SW","SampleId":"CW529_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L87" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.4">
@@ -3726,7 +3729,7 @@
       <c r="B88" t="s">
         <v>7</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88">
         <v>531</v>
       </c>
       <c r="D88" t="s">
@@ -3734,27 +3737,27 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
-        <v>CW531_2017</v>
+        <v>CW531_Bio_SW_2017</v>
       </c>
       <c r="F88">
         <v>1</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="4"/>
-        <v>CW531_2017</v>
+        <v>CW531_Bio_SW_2017</v>
       </c>
       <c r="I88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="5"/>
-        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":531,"Crop":"SW","SampleId":"CW531_2017","CropExists":1}</v>
+        <v>{"HarvestYear":2017,"FieldId":"CW","ID2":531,"Crop":"SW","SampleId":"CW531_Bio_SW_2017","CropExists":1}</v>
       </c>
       <c r="L88" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>